<commit_message>
Add chart for average incremental
</commit_message>
<xml_diff>
--- a/Test results/results.xlsx
+++ b/Test results/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10639193_polimi_it/Documents/papers/2020 distributed decision systems/tests/DaaSinFogComputing/Test results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D0CD4D-014A-984D-BA63-4DE34C1E9C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="6_{A99C741B-629A-1949-B398-3DD5D337BDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{702CAB9B-3C90-3146-9D4E-D475B8187B89}"/>
   <bookViews>
     <workbookView xWindow="-10680" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="8" xr2:uid="{C926F829-F91A-A246-AC1D-5E6E00D4B87F}"/>
   </bookViews>
@@ -24,16 +24,31 @@
     <sheet name="Comparison local vs global" sheetId="16" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'BoxPlot number of actions'!$B$2:$KO$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'BoxPlot number of actions'!$B$3:$KO$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'BoxPlot number of actions'!$B$4:$KO$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'BoxPlot number of actions'!$B$5:$KO$5</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'BoxPlot number of actions'!$B$6:$KO$6</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'BoxPlot number of actions'!$B$2:$CW$2</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'BoxPlot number of actions'!$B$3:$CW$3</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'BoxPlot number of actions'!$B$4:$CW$4</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'BoxPlot number of actions'!$B$5:$CW$5</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'BoxPlot number of actions'!$B$6:$CW$6</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Incremental '!$A$5:$A$14</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Incremental '!$C$5:$C$14</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Incremental '!$A$5:$A$14</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Incremental '!$C$5:$C$14</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'Incremental '!$F$5:$F$14</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'Incremental '!$I$5:$I$14</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'Incremental '!$L$5:$L$14</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'BoxPlot number of actions'!$B$2:$CW$2</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'BoxPlot number of actions'!$B$3:$CW$3</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'BoxPlot number of actions'!$B$4:$CW$4</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'BoxPlot number of actions'!$B$5:$CW$5</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'BoxPlot number of actions'!$B$6:$CW$6</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Incremental '!$F$5:$F$14</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'BoxPlot number of actions'!$B$2:$KO$2</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'BoxPlot number of actions'!$B$3:$KO$3</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'BoxPlot number of actions'!$B$4:$KO$4</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'BoxPlot number of actions'!$B$5:$KO$5</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'BoxPlot number of actions'!$B$6:$KO$6</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Incremental '!$I$5:$I$14</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Incremental '!$L$5:$L$14</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Incremental '!$A$5:$A$14</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Incremental '!$C$5:$C$14</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Incremental '!$F$5:$F$14</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Incremental '!$I$5:$I$14</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Incremental '!$L$5:$L$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -76,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="30">
   <si>
     <t>batch</t>
   </si>
@@ -97,9 +112,6 @@
   </si>
   <si>
     <t>average per number of nodes</t>
-  </si>
-  <si>
-    <t>avg</t>
   </si>
   <si>
     <t>Number of Full nodes</t>
@@ -135,19 +147,10 @@
     <t>Global decision</t>
   </si>
   <si>
-    <t>global</t>
-  </si>
-  <si>
     <t>batch 1</t>
   </si>
   <si>
     <t>batch 2</t>
-  </si>
-  <si>
-    <t>std dev</t>
-  </si>
-  <si>
-    <t>variance</t>
   </si>
   <si>
     <t>batch 3</t>
@@ -163,6 +166,21 @@
   </si>
   <si>
     <t>Local decision:</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>number of nodes</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>Variance</t>
   </si>
 </sst>
 </file>
@@ -219,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -289,11 +307,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -307,6 +343,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2565,6 +2607,475 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
+              <a:t>Incremental Addition of full nodes - Average</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1920" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Incremental '!$A$5:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Incremental '!$L$5:$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.333333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F8EC-4C4E-A95C-8516C987A3A4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="440780176"/>
+        <c:axId val="440781856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="440780176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440781856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="440781856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of adaptation actions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="440780176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1600"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1920" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
               <a:t>Average number of adaptation actions per configuration</a:t>
             </a:r>
           </a:p>
@@ -3218,7 +3729,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -3756,7 +4267,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -4312,27 +4823,27 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.0</cx:f>
+        <cx:f dir="row">_xlchart.v1.20</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.1</cx:f>
+        <cx:f dir="row">_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.2</cx:f>
+        <cx:f dir="row">_xlchart.v1.22</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.3</cx:f>
+        <cx:f dir="row">_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.4</cx:f>
+        <cx:f dir="row">_xlchart.v1.24</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4542,27 +5053,27 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.5</cx:f>
+        <cx:f dir="row">_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.6</cx:f>
+        <cx:f dir="row">_xlchart.v1.16</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.7</cx:f>
+        <cx:f dir="row">_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.8</cx:f>
+        <cx:f dir="row">_xlchart.v1.18</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.9</cx:f>
+        <cx:f dir="row">_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5087,6 +5598,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -6597,6 +7148,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7111,7 +8165,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7626,7 +8680,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8129,7 +9183,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8632,7 +9686,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9247,6 +10301,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>234949</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>226482</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E411E6FF-AE18-34F5-2390-1EF84A5225EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9845,7 +10935,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -9875,7 +10965,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
@@ -14330,51 +15420,57 @@
   <dimension ref="A3:AA18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="313" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.83203125" customWidth="1"/>
     <col min="15" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
+    <row r="3" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
+      <c r="G4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="J4" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="18" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" t="s">
-        <v>26</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -14392,25 +15488,27 @@
       <c r="A5">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>36</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="13">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="10">
         <v>34</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="9">
         <v>19</v>
       </c>
-      <c r="I5">
+      <c r="G5" s="13"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="9">
         <v>5</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="13">
         <v>0</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="10">
         <v>2</v>
       </c>
       <c r="L5">
@@ -14422,31 +15520,31 @@
       <c r="A6">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="9">
         <v>35</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="13">
         <v>4</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="10">
         <v>28</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="9">
         <v>9</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="13">
         <v>1</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="10">
         <v>4</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="9">
         <v>7</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="13">
         <v>2</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="10">
         <v>5</v>
       </c>
       <c r="L6">
@@ -14470,25 +15568,27 @@
       <c r="A7">
         <v>13</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
         <v>31</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="13">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="E7" s="10"/>
+      <c r="F7" s="9">
         <v>52</v>
       </c>
-      <c r="H7">
+      <c r="G7" s="13"/>
+      <c r="H7" s="10">
         <v>3</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="9">
         <v>16</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="13">
         <v>2</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="10">
         <v>7</v>
       </c>
       <c r="L7">
@@ -14512,22 +15612,25 @@
       <c r="A8">
         <v>14</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="9">
         <v>39</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="13">
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="E8" s="10"/>
+      <c r="F8" s="9">
         <v>28</v>
       </c>
-      <c r="I8">
+      <c r="G8" s="13"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="9">
         <v>22</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="13">
         <v>3</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="10">
         <v>8</v>
       </c>
       <c r="L8">
@@ -14551,22 +15654,25 @@
       <c r="A9">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="9">
         <v>36</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="13">
         <v>3</v>
       </c>
-      <c r="F9">
+      <c r="E9" s="10"/>
+      <c r="F9" s="9">
         <v>25</v>
       </c>
-      <c r="I9">
+      <c r="G9" s="13"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="9">
         <v>16</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="13">
         <v>3</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="10">
         <v>7</v>
       </c>
       <c r="L9">
@@ -14578,22 +15684,25 @@
       <c r="A10">
         <v>16</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="9">
         <v>33</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="13">
         <v>5</v>
       </c>
-      <c r="F10">
+      <c r="E10" s="10"/>
+      <c r="F10" s="9">
         <v>17</v>
       </c>
-      <c r="I10">
+      <c r="G10" s="13"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="9">
         <v>70</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="13">
         <v>10</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="10">
         <v>45</v>
       </c>
       <c r="L10">
@@ -14605,22 +15714,25 @@
       <c r="A11">
         <v>17</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="9">
         <v>16</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="13">
         <v>1</v>
       </c>
-      <c r="F11">
+      <c r="E11" s="10"/>
+      <c r="F11" s="9">
         <v>46</v>
       </c>
-      <c r="I11">
+      <c r="G11" s="13"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="9">
         <v>71</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="13">
         <v>6</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="10">
         <v>63</v>
       </c>
       <c r="L11">
@@ -14632,18 +15744,23 @@
       <c r="A12">
         <v>18</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="9">
         <v>21</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="13">
         <v>5</v>
       </c>
-      <c r="F12">
+      <c r="E12" s="10"/>
+      <c r="F12" s="9">
         <v>12</v>
       </c>
-      <c r="I12">
+      <c r="G12" s="13"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="9">
         <v>9</v>
       </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="10"/>
       <c r="L12">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -14653,39 +15770,49 @@
       <c r="A13">
         <v>19</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="9">
         <v>25</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="13">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="E13" s="10"/>
+      <c r="F13" s="9">
         <v>8</v>
       </c>
-      <c r="I13">
+      <c r="G13" s="13"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="9">
         <v>14</v>
       </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="10"/>
       <c r="L13">
         <f t="shared" si="0"/>
         <v>15.666666666666666</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="11">
         <v>29</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="14">
         <v>3</v>
       </c>
-      <c r="F14">
+      <c r="E14" s="12"/>
+      <c r="F14" s="11">
         <v>10</v>
       </c>
-      <c r="I14">
+      <c r="G14" s="14"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="11">
         <v>7</v>
       </c>
+      <c r="J14" s="14"/>
+      <c r="K14" s="12"/>
       <c r="L14">
         <f t="shared" si="0"/>
         <v>15.333333333333334</v>
@@ -14693,7 +15820,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C15">
         <f>AVERAGE(C5:C14)</f>
@@ -14710,7 +15837,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <f>STDEV(C5:C15)</f>
@@ -14727,7 +15854,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <f>_xlfn.VAR.P(C5:C14)</f>
@@ -14744,7 +15871,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>12</v>
@@ -14785,7 +15912,7 @@
         <v>4</v>
       </c>
       <c r="GT1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:301" x14ac:dyDescent="0.2">
@@ -20860,7 +21987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D890983F-CDEF-7440-9083-3C6F46E5832B}">
   <dimension ref="A1:AA159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
@@ -20874,7 +22001,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H1">
         <v>3</v>
@@ -21103,10 +22230,10 @@
     </row>
     <row r="9" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -21128,10 +22255,10 @@
         <v>0</v>
       </c>
       <c r="Z10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA10" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="AA10" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
@@ -21159,11 +22286,11 @@
         <v>3.2863353450309969</v>
       </c>
       <c r="Z11" s="9">
-        <f>AVERAGE(U2,U10,U17,U25)</f>
+        <f t="shared" ref="Z11:AA15" si="2">AVERAGE(U2,U10,U17,U25)</f>
         <v>0</v>
       </c>
       <c r="AA11" s="10">
-        <f>AVERAGE(V2,V10,V17,V25)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -21207,11 +22334,11 @@
         <v>10.764654094664529</v>
       </c>
       <c r="Z12" s="9">
-        <f>AVERAGE(U3,U11,U18,U26)</f>
+        <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
       <c r="AA12" s="10">
-        <f>AVERAGE(V3,V11,V18,V26)</f>
+        <f t="shared" si="2"/>
         <v>2.6787532701676051</v>
       </c>
     </row>
@@ -21270,11 +22397,11 @@
         <v>19.704483415371911</v>
       </c>
       <c r="Z13" s="9">
-        <f>AVERAGE(U4,U12,U19,U27)</f>
+        <f t="shared" si="2"/>
         <v>17.975000000000001</v>
       </c>
       <c r="AA13" s="10">
-        <f>AVERAGE(V4,V12,V19,V27)</f>
+        <f t="shared" si="2"/>
         <v>13.281556788193761</v>
       </c>
     </row>
@@ -21348,27 +22475,27 @@
         <v>17.882658462438144</v>
       </c>
       <c r="Z14" s="9">
-        <f>AVERAGE(U5,U13,U20,U28)</f>
+        <f t="shared" si="2"/>
         <v>19.133333333333333</v>
       </c>
       <c r="AA14" s="10">
-        <f>AVERAGE(V5,V13,V20,V28)</f>
+        <f t="shared" si="2"/>
         <v>14.171104670267828</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="Z15" s="11">
-        <f>AVERAGE(U6,U14,U21,U29)</f>
+        <f t="shared" si="2"/>
         <v>21.587500000000002</v>
       </c>
       <c r="AA15" s="12">
-        <f>AVERAGE(V6,V14,V21,V29)</f>
+        <f t="shared" si="2"/>
         <v>12.902906443315221</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
@@ -21386,7 +22513,7 @@
         <v>0</v>
       </c>
       <c r="V17">
-        <f t="shared" ref="V17:V21" si="2">STDEV(A17:T17)</f>
+        <f t="shared" ref="V17:V21" si="3">STDEV(A17:T17)</f>
         <v>0</v>
       </c>
     </row>
@@ -21411,7 +22538,7 @@
         <v>1.2</v>
       </c>
       <c r="V18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3038404810405297</v>
       </c>
     </row>
@@ -21451,7 +22578,7 @@
         <v>21.7</v>
       </c>
       <c r="V19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.470760952339884</v>
       </c>
     </row>
@@ -21506,7 +22633,7 @@
         <v>13.266666666666667</v>
       </c>
       <c r="V20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.9100718367489051</v>
       </c>
     </row>
@@ -21576,13 +22703,13 @@
         <v>17.8</v>
       </c>
       <c r="V21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.8887865491184712</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
@@ -21600,7 +22727,7 @@
         <v>0</v>
       </c>
       <c r="V25">
-        <f t="shared" ref="V25:V29" si="3">STDEV(A25:T25)</f>
+        <f t="shared" ref="V25:V29" si="4">STDEV(A25:T25)</f>
         <v>0</v>
       </c>
     </row>
@@ -21625,7 +22752,7 @@
         <v>2.6</v>
       </c>
       <c r="V26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.2093613071762426</v>
       </c>
     </row>
@@ -21665,7 +22792,7 @@
         <v>16</v>
       </c>
       <c r="V27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14.712050993809275</v>
       </c>
     </row>
@@ -21720,7 +22847,7 @@
         <v>17.866666666666667</v>
       </c>
       <c r="V28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.195598111635924</v>
       </c>
     </row>
@@ -21790,7 +22917,7 @@
         <v>9.9</v>
       </c>
       <c r="V29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.471801180994035</v>
       </c>
     </row>
@@ -21808,10 +22935,10 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>